<commit_message>
CTDC diagnosis 13 scripts
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Trials_Filter_Diagnosis-AdenoCervix.xlsx
+++ b/InputFiles/TC01_Trials_Filter_Diagnosis-AdenoCervix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Automation\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C94AFC13-E767-4A8D-96EC-3A0192EFCE7F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A993829-AACD-4627-865E-9D9A0046336C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>WebExcel</t>
   </si>
@@ -57,27 +57,63 @@
     <t>TC03_Trials_Filter_Diagnosis-AdenoGastro_Neo4jData.xlsx</t>
   </si>
   <si>
-    <t>MATCH (ct:clinical_trial)&lt;--(a:arm)&lt;--(c:case)
-    WHERE c.diagnosis = "Adenocarcinoma of the cervix"
-WITH DISTINCT c, a, ct
-RETURN 
-    COALESCE(c.case_id, '') AS `Case ID`,
-    COALESCE(ct.clinical_trial_designation, '') AS `Trial Code`,
-    COALESCE(a.arm_id, '') AS `Arm`,
-    COALESCE(a.arm_drug, '') AS `Arm Treatment`,
-    COALESCE(c.disease, '') AS `Diagnosis`,
-    COALESCE(c.gender, '') AS `Gender`,
-    COALESCE(c.race, '') AS `Race`,
-    COALESCE(c.ethnicity, '') AS `Ethnicity`</t>
-  </si>
-  <si>
-    <t>MATCH (s:specimen)--&gt;(c:case)--&gt;(:arm)--&gt;(ct:clinical_trial)
-    WHERE c.diagnosis = "Adenocarcinoma of the cervix"
-OPTIONAL MATCH (f:file)--&gt;(:sequencing_assay)--&gt;(:nucleic_acid)--&gt;(s)
-RETURN 
-    COUNT(DISTINCT f) AS number_of_files,
-    COUNT(DISTINCT c.case_id) AS number_of_cases,
-    COUNT(DISTINCT ct.clinical_trial_designation) AS number_of_trials</t>
+    <t>FilesTab</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)
+OPTIONAL MATCH (f)-[*]-&gt;(a:arm)-[:of_trial]-&gt;(ct:clinical_trial)
+OPTIONAL MATCH (f)-[*]-&gt;(c:case)
+WITH f,a,ct,c
+   WHERE c.disease = "Adenocarcinoma of the cervix"
+RETURN
+    COUNT(DISTINCT ct.clinical_trial_designation) AS Trials,
+    COUNT(DISTINCT c.case_id) AS Cases,
+    COUNT(DISTINCT f) AS Files</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)
+OPTIONAL MATCH (f)-[*]-&gt;(a:arm)-[:of_trial]-&gt;(ct:clinical_trial)
+OPTIONAL MATCH (f)-[*]-&gt;(c:case)
+OPTIONAL MATCH (f)--&gt;(parent)
+WITH f,a,ct,c,parent
+ WHERE c.disease = "Adenocarcinoma of the cervix"
+WITH
+    f, parent, c, a, ct,
+    ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+    toInteger(floor(log(f.file_size)/log(1024))) as i,
+    2 as precision
+WITH
+    f, parent, c, a, ct,
+    f.file_size /(1024^i) AS value,
+    10^precision AS factor,
+    units[i] as unit
+WITH
+    f, parent, c, a, ct, unit,
+    round(factor * value)/factor AS size
+RETURN DISTINCT
+    f.file_name AS `File Name`,
+    head(labels(parent)) as Association,
+    f.file_description AS Description,
+    f.file_format AS `File Format`,
+    CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+    ct.clinical_trial_designation AS `Trial Code`,
+    a.arm_id AS Arm,
+    c.case_id AS `Case ID`</t>
+  </si>
+  <si>
+    <t>MATCH (c:case)
+ MATCH (c)-[:of_arm]-&gt;(a:arm)-[:of_trial]-&gt;(ct:clinical_trial)
+ MATCH (f:file)-[*]-&gt;(c)
+ WHERE c.disease = "Adenocarcinoma of the cervix"
+RETURN DISTINCT
+    c.case_id AS `Case ID`,
+     ct.clinical_trial_designation AS `Trial Code`,
+     a.arm_id AS Arm,
+      a.arm_drug AS `Arm Treatment`,
+c.disease AS Diagnosis,
+  c.gender AS Gender,
+    c.race AS Race,
+    c.ethnicity AS Ethnicity</t>
   </si>
 </sst>
 </file>
@@ -447,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,12 +514,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="180" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="195" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>9</v>
@@ -492,6 +528,23 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CTDC working fine locally
</commit_message>
<xml_diff>
--- a/InputFiles/TC01_Trials_Filter_Diagnosis-AdenoCervix.xlsx
+++ b/InputFiles/TC01_Trials_Filter_Diagnosis-AdenoCervix.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Automation\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A993829-AACD-4627-865E-9D9A0046336C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8566E333-A49B-47A0-AA6D-75E9ACEA1654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>